<commit_message>
Email for importing and exporting products
</commit_message>
<xml_diff>
--- a/Products.xlsx
+++ b/Products.xlsx
@@ -851,7 +851,7 @@
     </row>
     <row r="30">
       <c r="A30" s="0" t="n">
-        <v>15502502</v>
+        <v>15502503</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>1550</v>
@@ -860,13 +860,13 @@
         <v>25</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E30" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F30" s="0" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="G30" s="0" t="inlineStr">
         <is>
@@ -876,7 +876,7 @@
     </row>
     <row r="31">
       <c r="A31" s="0" t="n">
-        <v>15502503</v>
+        <v>15502504</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>1550</v>
@@ -885,13 +885,13 @@
         <v>25</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E31" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F31" s="0" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
       <c r="G31" s="0" t="inlineStr">
         <is>
@@ -901,7 +901,7 @@
     </row>
     <row r="32">
       <c r="A32" s="0" t="n">
-        <v>15502504</v>
+        <v>15502505</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>1550</v>
@@ -910,13 +910,13 @@
         <v>25</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E32" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F32" s="0" t="n">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="G32" s="0" t="inlineStr">
         <is>
@@ -926,7 +926,7 @@
     </row>
     <row r="33">
       <c r="A33" s="0" t="n">
-        <v>15502505</v>
+        <v>15502506</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>1550</v>
@@ -935,13 +935,13 @@
         <v>25</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E33" s="0" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F33" s="0" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="G33" s="0" t="inlineStr">
         <is>
@@ -951,7 +951,7 @@
     </row>
     <row r="34">
       <c r="A34" s="0" t="n">
-        <v>15502506</v>
+        <v>15502507</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>1550</v>
@@ -960,13 +960,13 @@
         <v>25</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E34" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F34" s="0" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="G34" s="0" t="inlineStr">
         <is>
@@ -976,7 +976,7 @@
     </row>
     <row r="35">
       <c r="A35" s="0" t="n">
-        <v>15502507</v>
+        <v>15502508</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>1550</v>
@@ -985,13 +985,13 @@
         <v>25</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E35" s="0" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F35" s="0" t="n">
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
       <c r="G35" s="0" t="inlineStr">
         <is>
@@ -1001,7 +1001,7 @@
     </row>
     <row r="36">
       <c r="A36" s="0" t="n">
-        <v>15502508</v>
+        <v>15502509</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>1550</v>
@@ -1010,13 +1010,13 @@
         <v>25</v>
       </c>
       <c r="D36" s="0" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E36" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F36" s="0" t="n">
-        <v>13.0</v>
+        <v>14.0</v>
       </c>
       <c r="G36" s="0" t="inlineStr">
         <is>
@@ -1026,22 +1026,22 @@
     </row>
     <row r="37">
       <c r="A37" s="0" t="n">
-        <v>15502509</v>
+        <v>1550251</v>
       </c>
       <c r="B37" s="0" t="n">
-        <v>1550</v>
+        <v>155</v>
       </c>
       <c r="C37" s="0" t="n">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="D37" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="E37" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="E37" s="0" t="n">
-        <v>4</v>
-      </c>
       <c r="F37" s="0" t="n">
-        <v>14.0</v>
+        <v>15.0</v>
       </c>
       <c r="G37" s="0" t="inlineStr">
         <is>
@@ -1051,22 +1051,22 @@
     </row>
     <row r="38">
       <c r="A38" s="0" t="n">
-        <v>1550251</v>
+        <v>15502511</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>155</v>
+        <v>1550</v>
       </c>
       <c r="C38" s="0" t="n">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="E38" s="0" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F38" s="0" t="n">
-        <v>15.0</v>
+        <v>16.0</v>
       </c>
       <c r="G38" s="0" t="inlineStr">
         <is>
@@ -1076,7 +1076,7 @@
     </row>
     <row r="39">
       <c r="A39" s="0" t="n">
-        <v>15502511</v>
+        <v>15502512</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>1550</v>
@@ -1085,13 +1085,13 @@
         <v>25</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E39" s="0" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F39" s="0" t="n">
-        <v>16.0</v>
+        <v>17.0</v>
       </c>
       <c r="G39" s="0" t="inlineStr">
         <is>
@@ -1101,7 +1101,7 @@
     </row>
     <row r="40">
       <c r="A40" s="0" t="n">
-        <v>15502512</v>
+        <v>15502513</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>1550</v>
@@ -1110,13 +1110,13 @@
         <v>25</v>
       </c>
       <c r="D40" s="0" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E40" s="0" t="n">
         <v>3</v>
       </c>
       <c r="F40" s="0" t="n">
-        <v>17.0</v>
+        <v>18.0</v>
       </c>
       <c r="G40" s="0" t="inlineStr">
         <is>
@@ -1126,7 +1126,7 @@
     </row>
     <row r="41">
       <c r="A41" s="0" t="n">
-        <v>15502513</v>
+        <v>15502514</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>1550</v>
@@ -1135,13 +1135,13 @@
         <v>25</v>
       </c>
       <c r="D41" s="0" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E41" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" s="0" t="n">
-        <v>18.0</v>
+        <v>19.0</v>
       </c>
       <c r="G41" s="0" t="inlineStr">
         <is>
@@ -1151,7 +1151,7 @@
     </row>
     <row r="42">
       <c r="A42" s="0" t="n">
-        <v>15502514</v>
+        <v>15502502</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>1550</v>
@@ -1160,13 +1160,13 @@
         <v>25</v>
       </c>
       <c r="D42" s="0" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="E42" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F42" s="0" t="n">
-        <v>19.0</v>
+        <v>7.0</v>
       </c>
       <c r="G42" s="0" t="inlineStr">
         <is>

</xml_diff>